<commit_message>
Wybranie ostatecznych danych -- wkoncu
</commit_message>
<xml_diff>
--- a/Projekt/Dane/Tabela_polaczona.xlsx
+++ b/Projekt/Dane/Tabela_polaczona.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arkadiusz Studia\Desktop\studia 4 semestr\Ekonometria\Projekt-laborki\Projekt-laborki\Projekt\Dane\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FED3642-328F-4B29-91F0-E4E9F98437D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C369A1-9B7D-4F68-9C04-A1E44FDFC02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="318">
   <si>
     <t>Nazwa</t>
   </si>
@@ -34,9 +34,6 @@
     <t>1,0</t>
   </si>
   <si>
-    <t>-1,19</t>
-  </si>
-  <si>
     <t>3,79</t>
   </si>
   <si>
@@ -52,9 +49,6 @@
     <t>1,7</t>
   </si>
   <si>
-    <t>-1,00</t>
-  </si>
-  <si>
     <t>3,32</t>
   </si>
   <si>
@@ -70,9 +64,6 @@
     <t>0,8</t>
   </si>
   <si>
-    <t>-0,27</t>
-  </si>
-  <si>
     <t>4,59</t>
   </si>
   <si>
@@ -88,9 +79,6 @@
     <t>5,5</t>
   </si>
   <si>
-    <t>-5,94</t>
-  </si>
-  <si>
     <t>4,84</t>
   </si>
   <si>
@@ -106,9 +94,6 @@
     <t>2,0</t>
   </si>
   <si>
-    <t>-3,85</t>
-  </si>
-  <si>
     <t>4,36</t>
   </si>
   <si>
@@ -124,9 +109,6 @@
     <t>0,3</t>
   </si>
   <si>
-    <t>-1,90</t>
-  </si>
-  <si>
     <t>3,47</t>
   </si>
   <si>
@@ -142,9 +124,6 @@
     <t>2,4</t>
   </si>
   <si>
-    <t>-5,18</t>
-  </si>
-  <si>
     <t>4,75</t>
   </si>
   <si>
@@ -160,9 +139,6 @@
     <t>4,5</t>
   </si>
   <si>
-    <t>-7,28</t>
-  </si>
-  <si>
     <t>5,45</t>
   </si>
   <si>
@@ -178,9 +154,6 @@
     <t>2,6</t>
   </si>
   <si>
-    <t>-9,00</t>
-  </si>
-  <si>
     <t>3,76</t>
   </si>
   <si>
@@ -196,9 +169,6 @@
     <t>4,4</t>
   </si>
   <si>
-    <t>-6,64</t>
-  </si>
-  <si>
     <t>6,65</t>
   </si>
   <si>
@@ -214,9 +184,6 @@
     <t>4,3</t>
   </si>
   <si>
-    <t>-7,88</t>
-  </si>
-  <si>
     <t>6,44</t>
   </si>
   <si>
@@ -229,9 +196,6 @@
     <t>8,0</t>
   </si>
   <si>
-    <t>-6,32</t>
-  </si>
-  <si>
     <t>6,84</t>
   </si>
   <si>
@@ -247,9 +211,6 @@
     <t>17,7</t>
   </si>
   <si>
-    <t>-10,16</t>
-  </si>
-  <si>
     <t>6,27</t>
   </si>
   <si>
@@ -265,9 +226,6 @@
     <t>9,2</t>
   </si>
   <si>
-    <t>-3,52</t>
-  </si>
-  <si>
     <t>7,96</t>
   </si>
   <si>
@@ -280,9 +238,6 @@
     <t>2,3</t>
   </si>
   <si>
-    <t>-6,38</t>
-  </si>
-  <si>
     <t>4,51</t>
   </si>
   <si>
@@ -295,9 +250,6 @@
     <t>1,2</t>
   </si>
   <si>
-    <t>-5,72</t>
-  </si>
-  <si>
     <t>5,95</t>
   </si>
   <si>
@@ -313,9 +265,6 @@
     <t>1,6</t>
   </si>
   <si>
-    <t>-3,93</t>
-  </si>
-  <si>
     <t>5,51</t>
   </si>
   <si>
@@ -331,9 +280,6 @@
     <t>3,3</t>
   </si>
   <si>
-    <t>-3,98</t>
-  </si>
-  <si>
     <t>5,22</t>
   </si>
   <si>
@@ -343,9 +289,6 @@
     <t>5021,32</t>
   </si>
   <si>
-    <t>-2,65</t>
-  </si>
-  <si>
     <t>6,12</t>
   </si>
   <si>
@@ -355,9 +298,6 @@
     <t>5021,43</t>
   </si>
   <si>
-    <t>-4,82</t>
-  </si>
-  <si>
     <t>4,9</t>
   </si>
   <si>
@@ -367,9 +307,6 @@
     <t>5119,01</t>
   </si>
   <si>
-    <t>0,66</t>
-  </si>
-  <si>
     <t>5,65</t>
   </si>
   <si>
@@ -379,9 +316,6 @@
     <t>6662,69</t>
   </si>
   <si>
-    <t>-2,79</t>
-  </si>
-  <si>
     <t>4,53</t>
   </si>
   <si>
@@ -394,9 +328,6 @@
     <t>2,1</t>
   </si>
   <si>
-    <t>-6,57</t>
-  </si>
-  <si>
     <t>7,20</t>
   </si>
   <si>
@@ -409,9 +340,6 @@
     <t>5020,01</t>
   </si>
   <si>
-    <t>-7,18</t>
-  </si>
-  <si>
     <t>5,34</t>
   </si>
   <si>
@@ -427,9 +355,6 @@
     <t>2,2</t>
   </si>
   <si>
-    <t>-6,74</t>
-  </si>
-  <si>
     <t>4,68</t>
   </si>
   <si>
@@ -439,9 +364,6 @@
     <t>5342,48</t>
   </si>
   <si>
-    <t>-5,01</t>
-  </si>
-  <si>
     <t>5,88</t>
   </si>
   <si>
@@ -454,9 +376,6 @@
     <t>8,5</t>
   </si>
   <si>
-    <t>-8,71</t>
-  </si>
-  <si>
     <t>5,61</t>
   </si>
   <si>
@@ -466,9 +385,6 @@
     <t>7106,37</t>
   </si>
   <si>
-    <t>-5,27</t>
-  </si>
-  <si>
     <t>7,66</t>
   </si>
   <si>
@@ -481,9 +397,6 @@
     <t>5420,04</t>
   </si>
   <si>
-    <t>-10,34</t>
-  </si>
-  <si>
     <t>5,80</t>
   </si>
   <si>
@@ -499,9 +412,6 @@
     <t>3,2</t>
   </si>
   <si>
-    <t>-1,80</t>
-  </si>
-  <si>
     <t>6,61</t>
   </si>
   <si>
@@ -511,9 +421,6 @@
     <t>6693,90</t>
   </si>
   <si>
-    <t>-2,02</t>
-  </si>
-  <si>
     <t>4,38</t>
   </si>
   <si>
@@ -529,9 +436,6 @@
     <t>1,8</t>
   </si>
   <si>
-    <t>-7,81</t>
-  </si>
-  <si>
     <t>5,73</t>
   </si>
   <si>
@@ -547,9 +451,6 @@
     <t>9,7</t>
   </si>
   <si>
-    <t>-5,22</t>
-  </si>
-  <si>
     <t>6,56</t>
   </si>
   <si>
@@ -565,9 +466,6 @@
     <t>3,8</t>
   </si>
   <si>
-    <t>-4,95</t>
-  </si>
-  <si>
     <t>5,82</t>
   </si>
   <si>
@@ -583,9 +481,6 @@
     <t>1,1</t>
   </si>
   <si>
-    <t>-5,79</t>
-  </si>
-  <si>
     <t>6,66</t>
   </si>
   <si>
@@ -601,9 +496,6 @@
     <t>1,5</t>
   </si>
   <si>
-    <t>-7,59</t>
-  </si>
-  <si>
     <t>4,85</t>
   </si>
   <si>
@@ -619,9 +511,6 @@
     <t>6,6</t>
   </si>
   <si>
-    <t>-6,14</t>
-  </si>
-  <si>
     <t>7,19</t>
   </si>
   <si>
@@ -634,9 +523,6 @@
     <t>4980,31</t>
   </si>
   <si>
-    <t>-4,43</t>
-  </si>
-  <si>
     <t>6,24</t>
   </si>
   <si>
@@ -649,9 +535,6 @@
     <t>0,4</t>
   </si>
   <si>
-    <t>1,96</t>
-  </si>
-  <si>
     <t>4,98</t>
   </si>
   <si>
@@ -661,9 +544,6 @@
     <t>5295,68</t>
   </si>
   <si>
-    <t>-4,31</t>
-  </si>
-  <si>
     <t>6,80</t>
   </si>
   <si>
@@ -676,9 +556,6 @@
     <t>3,5</t>
   </si>
   <si>
-    <t>-3,76</t>
-  </si>
-  <si>
     <t>5,48</t>
   </si>
   <si>
@@ -691,9 +568,6 @@
     <t>3,7</t>
   </si>
   <si>
-    <t>-3,43</t>
-  </si>
-  <si>
     <t>4,40</t>
   </si>
   <si>
@@ -706,9 +580,6 @@
     <t>4851,74</t>
   </si>
   <si>
-    <t>-1,61</t>
-  </si>
-  <si>
     <t>7,13</t>
   </si>
   <si>
@@ -718,9 +589,6 @@
     <t>4854,96</t>
   </si>
   <si>
-    <t>-6,31</t>
-  </si>
-  <si>
     <t>6,54</t>
   </si>
   <si>
@@ -733,9 +601,6 @@
     <t>4838,42</t>
   </si>
   <si>
-    <t>-5,99</t>
-  </si>
-  <si>
     <t>6,10</t>
   </si>
   <si>
@@ -748,9 +613,6 @@
     <t>5421,76</t>
   </si>
   <si>
-    <t>-5,78</t>
-  </si>
-  <si>
     <t>5,91</t>
   </si>
   <si>
@@ -763,9 +625,6 @@
     <t>5209,89</t>
   </si>
   <si>
-    <t>-7,03</t>
-  </si>
-  <si>
     <t>4,88</t>
   </si>
   <si>
@@ -778,9 +637,6 @@
     <t>6062,04</t>
   </si>
   <si>
-    <t>-9,96</t>
-  </si>
-  <si>
     <t>5,09</t>
   </si>
   <si>
@@ -796,9 +652,6 @@
     <t>79,6</t>
   </si>
   <si>
-    <t>-6,87</t>
-  </si>
-  <si>
     <t>4,70</t>
   </si>
   <si>
@@ -808,9 +661,6 @@
     <t>4996,58</t>
   </si>
   <si>
-    <t>-5,87</t>
-  </si>
-  <si>
     <t>5,26</t>
   </si>
   <si>
@@ -823,9 +673,6 @@
     <t>5078,74</t>
   </si>
   <si>
-    <t>-7,53</t>
-  </si>
-  <si>
     <t>6,1</t>
   </si>
   <si>
@@ -835,9 +682,6 @@
     <t>5319,61</t>
   </si>
   <si>
-    <t>-7,85</t>
-  </si>
-  <si>
     <t>5,93</t>
   </si>
   <si>
@@ -850,9 +694,6 @@
     <t>30,9</t>
   </si>
   <si>
-    <t>-8,54</t>
-  </si>
-  <si>
     <t>4,07</t>
   </si>
   <si>
@@ -865,9 +706,6 @@
     <t>4799,77</t>
   </si>
   <si>
-    <t>-7,30</t>
-  </si>
-  <si>
     <t>4,94</t>
   </si>
   <si>
@@ -880,9 +718,6 @@
     <t>4872,40</t>
   </si>
   <si>
-    <t>-8,87</t>
-  </si>
-  <si>
     <t>4,25</t>
   </si>
   <si>
@@ -907,9 +742,6 @@
     <t>4982,57</t>
   </si>
   <si>
-    <t>-6,96</t>
-  </si>
-  <si>
     <t>5,37</t>
   </si>
   <si>
@@ -922,9 +754,6 @@
     <t>4872,03</t>
   </si>
   <si>
-    <t>-5,31</t>
-  </si>
-  <si>
     <t>5,14</t>
   </si>
   <si>
@@ -937,9 +766,6 @@
     <t>4852,38</t>
   </si>
   <si>
-    <t>-5,41</t>
-  </si>
-  <si>
     <t>4,80</t>
   </si>
   <si>
@@ -952,9 +778,6 @@
     <t>5494,92</t>
   </si>
   <si>
-    <t>-1,93</t>
-  </si>
-  <si>
     <t>4,56</t>
   </si>
   <si>
@@ -967,9 +790,6 @@
     <t>5112,92</t>
   </si>
   <si>
-    <t>-4,66</t>
-  </si>
-  <si>
     <t>4,17</t>
   </si>
   <si>
@@ -982,9 +802,6 @@
     <t>0,6</t>
   </si>
   <si>
-    <t>-3,84</t>
-  </si>
-  <si>
     <t>5,85</t>
   </si>
   <si>
@@ -997,9 +814,6 @@
     <t>5505,78</t>
   </si>
   <si>
-    <t>-8,08</t>
-  </si>
-  <si>
     <t>8,02</t>
   </si>
   <si>
@@ -1012,9 +826,6 @@
     <t>5135,12</t>
   </si>
   <si>
-    <t>-6,05</t>
-  </si>
-  <si>
     <t>5,92</t>
   </si>
   <si>
@@ -1024,9 +835,6 @@
     <t>7687,58</t>
   </si>
   <si>
-    <t>-2,29</t>
-  </si>
-  <si>
     <t>3,43</t>
   </si>
   <si>
@@ -1039,9 +847,6 @@
     <t>0,7</t>
   </si>
   <si>
-    <t>-1,47</t>
-  </si>
-  <si>
     <t>3,50</t>
   </si>
   <si>
@@ -1054,9 +859,6 @@
     <t>6350,07</t>
   </si>
   <si>
-    <t>-1,88</t>
-  </si>
-  <si>
     <t>3,41</t>
   </si>
   <si>
@@ -1081,9 +883,6 @@
     <t>5,1</t>
   </si>
   <si>
-    <t>-4,78</t>
-  </si>
-  <si>
     <t>4,28</t>
   </si>
   <si>
@@ -1099,9 +898,6 @@
     <t>16,5</t>
   </si>
   <si>
-    <t>-6,21</t>
-  </si>
-  <si>
     <t>3,54</t>
   </si>
   <si>
@@ -1117,9 +913,6 @@
     <t>13,5</t>
   </si>
   <si>
-    <t>-6,77</t>
-  </si>
-  <si>
     <t>3,92</t>
   </si>
   <si>
@@ -1135,9 +928,6 @@
     <t>0,9</t>
   </si>
   <si>
-    <t>-4,48</t>
-  </si>
-  <si>
     <t>5,13</t>
   </si>
   <si>
@@ -1147,9 +937,6 @@
     <t>5864,86</t>
   </si>
   <si>
-    <t>-6,16</t>
-  </si>
-  <si>
     <t>3,82</t>
   </si>
   <si>
@@ -1171,9 +958,6 @@
     <t>dwutlenek siarki na 1 mieszkańca</t>
   </si>
   <si>
-    <t>przyrost naturalny na 1000 ludności</t>
-  </si>
-  <si>
     <t>nakłady inwestycyjne na 1 mieszkańca</t>
   </si>
   <si>
@@ -1187,6 +971,9 @@
   </si>
   <si>
     <t>Zgłoszenia wynalazków w UPRP na 1 mln mieszkańców</t>
+  </si>
+  <si>
+    <t>przestępstwa stwierdzone przez Policję ogółem na 1000 mieszkańców</t>
   </si>
 </sst>
 </file>
@@ -1578,7 +1365,7 @@
   <dimension ref="A1:H76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,36 +1373,37 @@
     <col min="1" max="1" width="41.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" customWidth="1"/>
     <col min="6" max="6" width="15.140625" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>381</v>
+        <v>310</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>382</v>
+        <v>311</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>383</v>
+        <v>317</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>384</v>
+        <v>312</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>385</v>
+        <v>313</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>388</v>
+        <v>316</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>386</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1645,25 +1433,25 @@
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="3" t="s">
-        <v>377</v>
+        <v>306</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>380</v>
+        <v>309</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>378</v>
+        <v>307</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>387</v>
+        <v>315</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>379</v>
+        <v>308</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>378</v>
+        <v>307</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>378</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1676,1892 +1464,1892 @@
       <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
-        <v>4</v>
+      <c r="D4">
+        <v>14.73</v>
       </c>
       <c r="E4">
         <v>2944</v>
       </c>
       <c r="F4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G4">
         <v>43.3</v>
       </c>
       <c r="H4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
+      <c r="D5">
+        <v>23.88</v>
       </c>
       <c r="E5">
         <v>6055</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G5">
         <v>282.10000000000002</v>
       </c>
       <c r="H5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
+      <c r="D6">
+        <v>27.79</v>
       </c>
       <c r="E6">
         <v>2695</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G6">
         <v>43.1</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>17.399999999999999</v>
       </c>
       <c r="E7">
         <v>4635</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G7">
         <v>78</v>
       </c>
       <c r="H7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>28</v>
+        <v>23</v>
+      </c>
+      <c r="D8">
+        <v>21.83</v>
       </c>
       <c r="E8">
         <v>2825</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G8">
         <v>26.4</v>
       </c>
       <c r="H8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="D9">
+        <v>15.65</v>
       </c>
       <c r="E9">
         <v>2589</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G9">
         <v>26.4</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="D10">
+        <v>21.7</v>
       </c>
       <c r="E10">
         <v>5118</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="G10">
         <v>53</v>
       </c>
       <c r="H10" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" t="s">
-        <v>46</v>
+        <v>38</v>
+      </c>
+      <c r="D11">
+        <v>21.66</v>
       </c>
       <c r="E11">
         <v>2875</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G11">
         <v>45.2</v>
       </c>
       <c r="H11" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" t="s">
-        <v>52</v>
+        <v>43</v>
+      </c>
+      <c r="D12">
+        <v>18.61</v>
       </c>
       <c r="E12">
         <v>3252</v>
       </c>
       <c r="F12" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="G12">
         <v>217.2</v>
       </c>
       <c r="H12" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" t="s">
-        <v>58</v>
+        <v>48</v>
+      </c>
+      <c r="D13">
+        <v>24.84</v>
       </c>
       <c r="E13">
         <v>7665</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="G13">
         <v>305.7</v>
       </c>
       <c r="H13" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" t="s">
-        <v>64</v>
+        <v>53</v>
+      </c>
+      <c r="D14">
+        <v>46.95</v>
       </c>
       <c r="E14">
         <v>5655</v>
       </c>
       <c r="F14" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="G14">
         <v>150.19999999999999</v>
       </c>
       <c r="H14" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" t="s">
-        <v>69</v>
+        <v>57</v>
+      </c>
+      <c r="D15">
+        <v>21.26</v>
       </c>
       <c r="E15">
         <v>4494</v>
       </c>
       <c r="F15" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="G15">
         <v>22.9</v>
       </c>
       <c r="H15" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" t="s">
-        <v>75</v>
+        <v>62</v>
+      </c>
+      <c r="D16">
+        <v>36.15</v>
       </c>
       <c r="E16">
         <v>5157</v>
       </c>
       <c r="F16" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="G16">
         <v>16.7</v>
       </c>
       <c r="H16" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D17" t="s">
-        <v>81</v>
+        <v>67</v>
+      </c>
+      <c r="D17">
+        <v>19.100000000000001</v>
       </c>
       <c r="E17">
         <v>7001</v>
       </c>
       <c r="F17" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="G17">
         <v>35.5</v>
       </c>
       <c r="H17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" t="s">
-        <v>86</v>
+        <v>71</v>
+      </c>
+      <c r="D18">
+        <v>30.18</v>
       </c>
       <c r="E18">
         <v>5661</v>
       </c>
       <c r="F18" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="G18">
         <v>18.600000000000001</v>
       </c>
       <c r="H18" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
-      </c>
-      <c r="D19" t="s">
-        <v>91</v>
+        <v>75</v>
+      </c>
+      <c r="D19">
+        <v>25.9</v>
       </c>
       <c r="E19">
         <v>4815</v>
       </c>
       <c r="F19" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="G19">
         <v>45.7</v>
       </c>
       <c r="H19" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
-      </c>
-      <c r="D20" t="s">
-        <v>97</v>
+        <v>80</v>
+      </c>
+      <c r="D20">
+        <v>18.02</v>
       </c>
       <c r="E20">
         <v>5641</v>
       </c>
       <c r="F20" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="G20">
         <v>45.6</v>
       </c>
       <c r="H20" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C21" t="s">
-        <v>102</v>
-      </c>
-      <c r="D21" t="s">
-        <v>103</v>
+        <v>85</v>
+      </c>
+      <c r="D21">
+        <v>19.37</v>
       </c>
       <c r="E21">
         <v>4265</v>
       </c>
       <c r="F21" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="G21">
         <v>31.2</v>
       </c>
       <c r="H21" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="B22" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" t="s">
-        <v>107</v>
+        <v>23</v>
+      </c>
+      <c r="D22">
+        <v>16.489999999999998</v>
       </c>
       <c r="E22">
         <v>4504</v>
       </c>
       <c r="F22" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="G22">
         <v>34.4</v>
       </c>
       <c r="H22" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="B23" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" t="s">
-        <v>111</v>
+        <v>43</v>
+      </c>
+      <c r="D23">
+        <v>17.98</v>
       </c>
       <c r="E23">
         <v>4317</v>
       </c>
       <c r="F23" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="G23">
         <v>22.5</v>
       </c>
       <c r="H23" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="B24" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C24" t="s">
         <v>3</v>
       </c>
-      <c r="D24" t="s">
-        <v>115</v>
+      <c r="D24">
+        <v>17.48</v>
       </c>
       <c r="E24">
         <v>6385</v>
       </c>
       <c r="F24" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="G24">
         <v>69.5</v>
       </c>
       <c r="H24" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="B25" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" t="s">
-        <v>119</v>
+        <v>23</v>
+      </c>
+      <c r="D25">
+        <v>26.66</v>
       </c>
       <c r="E25">
         <v>8983</v>
       </c>
       <c r="F25" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="G25">
         <v>324.10000000000002</v>
       </c>
       <c r="H25" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="B26" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="C26" t="s">
-        <v>123</v>
-      </c>
-      <c r="D26" t="s">
-        <v>124</v>
+        <v>101</v>
+      </c>
+      <c r="D26">
+        <v>21.7</v>
       </c>
       <c r="E26">
         <v>2731</v>
       </c>
       <c r="F26" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="G26">
         <v>48.7</v>
       </c>
       <c r="H26" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="B27" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" t="s">
-        <v>129</v>
+        <v>33</v>
+      </c>
+      <c r="D27">
+        <v>22.36</v>
       </c>
       <c r="E27">
         <v>3125</v>
       </c>
       <c r="F27" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="G27">
         <v>17.3</v>
       </c>
       <c r="H27" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="B28" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="C28" t="s">
-        <v>134</v>
-      </c>
-      <c r="D28" t="s">
-        <v>135</v>
+        <v>110</v>
+      </c>
+      <c r="D28">
+        <v>31.28</v>
       </c>
       <c r="E28">
         <v>5429</v>
       </c>
       <c r="F28" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="G28">
         <v>283.2</v>
       </c>
       <c r="H28" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="B29" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="C29" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29" t="s">
-        <v>139</v>
+        <v>15</v>
+      </c>
+      <c r="D29">
+        <v>21.56</v>
       </c>
       <c r="E29">
         <v>8220</v>
       </c>
       <c r="F29" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="G29">
         <v>13.8</v>
       </c>
       <c r="H29" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="B30" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="C30" t="s">
-        <v>143</v>
-      </c>
-      <c r="D30" t="s">
-        <v>144</v>
+        <v>117</v>
+      </c>
+      <c r="D30">
+        <v>34.78</v>
       </c>
       <c r="E30">
         <v>6209</v>
       </c>
       <c r="F30" t="s">
-        <v>145</v>
+        <v>118</v>
       </c>
       <c r="G30">
         <v>22.1</v>
       </c>
       <c r="H30" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
       <c r="B31" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="C31" t="s">
-        <v>112</v>
-      </c>
-      <c r="D31" t="s">
-        <v>148</v>
+        <v>92</v>
+      </c>
+      <c r="D31">
+        <v>33.159999999999997</v>
       </c>
       <c r="E31">
         <v>8995</v>
       </c>
       <c r="F31" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="G31">
         <v>16.100000000000001</v>
       </c>
       <c r="H31" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="B32" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
-      </c>
-      <c r="D32" t="s">
-        <v>153</v>
+        <v>75</v>
+      </c>
+      <c r="D32">
+        <v>26.08</v>
       </c>
       <c r="E32">
         <v>3833</v>
       </c>
       <c r="F32" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="G32">
         <v>11.3</v>
       </c>
       <c r="H32" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="B33" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="C33" t="s">
-        <v>158</v>
-      </c>
-      <c r="D33" t="s">
-        <v>159</v>
+        <v>129</v>
+      </c>
+      <c r="D33">
+        <v>18.86</v>
       </c>
       <c r="E33">
         <v>10145</v>
       </c>
       <c r="F33" t="s">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="G33">
         <v>47.6</v>
       </c>
       <c r="H33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
       <c r="B34" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="C34" t="s">
         <v>3</v>
       </c>
-      <c r="D34" t="s">
-        <v>163</v>
+      <c r="D34">
+        <v>30.38</v>
       </c>
       <c r="E34">
         <v>7303</v>
       </c>
       <c r="F34" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
       <c r="G34">
         <v>294.3</v>
       </c>
       <c r="H34" t="s">
-        <v>165</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>166</v>
+        <v>135</v>
       </c>
       <c r="B35" t="s">
-        <v>167</v>
+        <v>136</v>
       </c>
       <c r="C35" t="s">
-        <v>168</v>
-      </c>
-      <c r="D35" t="s">
-        <v>169</v>
+        <v>137</v>
+      </c>
+      <c r="D35">
+        <v>18.5</v>
       </c>
       <c r="E35">
         <v>3691</v>
       </c>
       <c r="F35" t="s">
-        <v>170</v>
+        <v>138</v>
       </c>
       <c r="G35">
         <v>5.6</v>
       </c>
       <c r="H35" t="s">
-        <v>171</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
       <c r="B36" t="s">
-        <v>173</v>
+        <v>141</v>
       </c>
       <c r="C36" t="s">
-        <v>174</v>
-      </c>
-      <c r="D36" t="s">
-        <v>175</v>
+        <v>142</v>
+      </c>
+      <c r="D36">
+        <v>17.96</v>
       </c>
       <c r="E36">
         <v>4851</v>
       </c>
       <c r="F36" t="s">
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="G36">
         <v>55.5</v>
       </c>
       <c r="H36" t="s">
-        <v>177</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>178</v>
+        <v>145</v>
       </c>
       <c r="B37" t="s">
-        <v>179</v>
+        <v>146</v>
       </c>
       <c r="C37" t="s">
-        <v>180</v>
-      </c>
-      <c r="D37" t="s">
-        <v>181</v>
+        <v>147</v>
+      </c>
+      <c r="D37">
+        <v>22.97</v>
       </c>
       <c r="E37">
         <v>4339</v>
       </c>
       <c r="F37" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
       <c r="G37">
         <v>102.7</v>
       </c>
       <c r="H37" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="B38" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
       <c r="C38" t="s">
-        <v>186</v>
-      </c>
-      <c r="D38" t="s">
-        <v>187</v>
+        <v>152</v>
+      </c>
+      <c r="D38">
+        <v>16.75</v>
       </c>
       <c r="E38">
         <v>2988</v>
       </c>
       <c r="F38" t="s">
-        <v>188</v>
+        <v>153</v>
       </c>
       <c r="G38">
         <v>29.2</v>
       </c>
       <c r="H38" t="s">
-        <v>189</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>190</v>
+        <v>155</v>
       </c>
       <c r="B39" t="s">
-        <v>191</v>
+        <v>156</v>
       </c>
       <c r="C39" t="s">
-        <v>192</v>
-      </c>
-      <c r="D39" t="s">
-        <v>193</v>
+        <v>157</v>
+      </c>
+      <c r="D39">
+        <v>21.59</v>
       </c>
       <c r="E39">
         <v>5360</v>
       </c>
       <c r="F39" t="s">
-        <v>194</v>
+        <v>158</v>
       </c>
       <c r="G39">
         <v>14.5</v>
       </c>
       <c r="H39" t="s">
-        <v>195</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="B40" t="s">
-        <v>197</v>
+        <v>161</v>
       </c>
       <c r="C40" t="s">
-        <v>198</v>
-      </c>
-      <c r="D40" t="s">
-        <v>199</v>
+        <v>162</v>
+      </c>
+      <c r="D40">
+        <v>18.059999999999999</v>
       </c>
       <c r="E40">
         <v>3233</v>
       </c>
       <c r="F40" t="s">
-        <v>200</v>
+        <v>163</v>
       </c>
       <c r="G40">
         <v>20</v>
       </c>
       <c r="H40" t="s">
-        <v>201</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="B41" t="s">
-        <v>203</v>
+        <v>166</v>
       </c>
       <c r="C41" t="s">
-        <v>102</v>
-      </c>
-      <c r="D41" t="s">
-        <v>204</v>
+        <v>85</v>
+      </c>
+      <c r="D41">
+        <v>17.07</v>
       </c>
       <c r="E41">
         <v>3440</v>
       </c>
       <c r="F41" t="s">
-        <v>205</v>
+        <v>167</v>
       </c>
       <c r="G41">
         <v>5.5</v>
       </c>
       <c r="H41" t="s">
-        <v>171</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>206</v>
+        <v>168</v>
       </c>
       <c r="B42" t="s">
-        <v>207</v>
+        <v>169</v>
       </c>
       <c r="C42" t="s">
-        <v>208</v>
-      </c>
-      <c r="D42" t="s">
-        <v>209</v>
+        <v>170</v>
+      </c>
+      <c r="D42">
+        <v>18.45</v>
       </c>
       <c r="E42">
         <v>3629</v>
       </c>
       <c r="F42" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="G42">
         <v>25.6</v>
       </c>
       <c r="H42" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>211</v>
+        <v>172</v>
       </c>
       <c r="B43" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="C43" t="s">
-        <v>85</v>
-      </c>
-      <c r="D43" t="s">
-        <v>213</v>
+        <v>71</v>
+      </c>
+      <c r="D43">
+        <v>19.41</v>
       </c>
       <c r="E43">
         <v>3846</v>
       </c>
       <c r="F43" t="s">
-        <v>214</v>
+        <v>174</v>
       </c>
       <c r="G43">
         <v>27.7</v>
       </c>
       <c r="H43" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>215</v>
+        <v>175</v>
       </c>
       <c r="B44" t="s">
-        <v>216</v>
+        <v>176</v>
       </c>
       <c r="C44" t="s">
-        <v>217</v>
-      </c>
-      <c r="D44" t="s">
-        <v>218</v>
+        <v>177</v>
+      </c>
+      <c r="D44">
+        <v>18.46</v>
       </c>
       <c r="E44">
         <v>3170</v>
       </c>
       <c r="F44" t="s">
-        <v>219</v>
+        <v>178</v>
       </c>
       <c r="G44">
         <v>38.1</v>
       </c>
       <c r="H44" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>220</v>
+        <v>179</v>
       </c>
       <c r="B45" t="s">
-        <v>221</v>
+        <v>180</v>
       </c>
       <c r="C45" t="s">
-        <v>222</v>
-      </c>
-      <c r="D45" t="s">
-        <v>223</v>
+        <v>181</v>
+      </c>
+      <c r="D45">
+        <v>28.86</v>
       </c>
       <c r="E45">
         <v>8545</v>
       </c>
       <c r="F45" t="s">
-        <v>224</v>
+        <v>182</v>
       </c>
       <c r="G45">
         <v>192.4</v>
       </c>
       <c r="H45" t="s">
-        <v>225</v>
+        <v>183</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>226</v>
+        <v>184</v>
       </c>
       <c r="B46" t="s">
-        <v>227</v>
+        <v>185</v>
       </c>
       <c r="C46" t="s">
-        <v>15</v>
-      </c>
-      <c r="D46" t="s">
-        <v>228</v>
+        <v>13</v>
+      </c>
+      <c r="D46">
+        <v>16.100000000000001</v>
       </c>
       <c r="E46">
         <v>2798</v>
       </c>
       <c r="F46" t="s">
-        <v>229</v>
+        <v>186</v>
       </c>
       <c r="G46">
         <v>17.899999999999999</v>
       </c>
       <c r="H46" t="s">
-        <v>171</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>230</v>
+        <v>187</v>
       </c>
       <c r="B47" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="C47" t="s">
-        <v>51</v>
-      </c>
-      <c r="D47" t="s">
-        <v>232</v>
+        <v>43</v>
+      </c>
+      <c r="D47">
+        <v>19.89</v>
       </c>
       <c r="E47">
         <v>2785</v>
       </c>
       <c r="F47" t="s">
-        <v>233</v>
+        <v>189</v>
       </c>
       <c r="G47">
         <v>27.7</v>
       </c>
       <c r="H47" t="s">
-        <v>234</v>
+        <v>190</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>235</v>
+        <v>191</v>
       </c>
       <c r="B48" t="s">
-        <v>236</v>
+        <v>192</v>
       </c>
       <c r="C48" t="s">
-        <v>192</v>
-      </c>
-      <c r="D48" t="s">
-        <v>237</v>
+        <v>157</v>
+      </c>
+      <c r="D48">
+        <v>17.850000000000001</v>
       </c>
       <c r="E48">
         <v>2861</v>
       </c>
       <c r="F48" t="s">
-        <v>238</v>
+        <v>193</v>
       </c>
       <c r="G48">
         <v>32.6</v>
       </c>
       <c r="H48" t="s">
-        <v>239</v>
+        <v>194</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>240</v>
+        <v>195</v>
       </c>
       <c r="B49" t="s">
-        <v>241</v>
+        <v>196</v>
       </c>
       <c r="C49" t="s">
-        <v>99</v>
-      </c>
-      <c r="D49" t="s">
-        <v>242</v>
+        <v>82</v>
+      </c>
+      <c r="D49">
+        <v>17.41</v>
       </c>
       <c r="E49">
         <v>4502</v>
       </c>
       <c r="F49" t="s">
-        <v>243</v>
+        <v>197</v>
       </c>
       <c r="G49">
         <v>51.8</v>
       </c>
       <c r="H49" t="s">
-        <v>244</v>
+        <v>198</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>245</v>
+        <v>199</v>
       </c>
       <c r="B50" t="s">
-        <v>246</v>
+        <v>200</v>
       </c>
       <c r="C50" t="s">
-        <v>158</v>
-      </c>
-      <c r="D50" t="s">
-        <v>247</v>
+        <v>129</v>
+      </c>
+      <c r="D50">
+        <v>17.71</v>
       </c>
       <c r="E50">
         <v>4722</v>
       </c>
       <c r="F50" t="s">
-        <v>248</v>
+        <v>201</v>
       </c>
       <c r="G50">
         <v>76.599999999999994</v>
       </c>
       <c r="H50" t="s">
-        <v>249</v>
+        <v>202</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>250</v>
+        <v>203</v>
       </c>
       <c r="B51" t="s">
-        <v>251</v>
+        <v>204</v>
       </c>
       <c r="C51" t="s">
-        <v>165</v>
-      </c>
-      <c r="D51" t="s">
-        <v>252</v>
+        <v>134</v>
+      </c>
+      <c r="D51">
+        <v>24.7</v>
       </c>
       <c r="E51">
         <v>4950</v>
       </c>
       <c r="F51" t="s">
-        <v>253</v>
+        <v>205</v>
       </c>
       <c r="G51">
         <v>191.4</v>
       </c>
       <c r="H51" t="s">
-        <v>254</v>
+        <v>206</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>255</v>
+        <v>207</v>
       </c>
       <c r="B52" t="s">
-        <v>256</v>
+        <v>208</v>
       </c>
       <c r="C52" t="s">
-        <v>257</v>
-      </c>
-      <c r="D52" t="s">
-        <v>258</v>
+        <v>209</v>
+      </c>
+      <c r="D52">
+        <v>16.989999999999998</v>
       </c>
       <c r="E52">
         <v>4217</v>
       </c>
       <c r="F52" t="s">
-        <v>259</v>
+        <v>210</v>
       </c>
       <c r="G52">
         <v>31.9</v>
       </c>
       <c r="H52" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>260</v>
+        <v>211</v>
       </c>
       <c r="B53" t="s">
-        <v>261</v>
+        <v>212</v>
       </c>
       <c r="C53" t="s">
-        <v>12</v>
-      </c>
-      <c r="D53" t="s">
-        <v>262</v>
+        <v>10</v>
+      </c>
+      <c r="D53">
+        <v>36.200000000000003</v>
       </c>
       <c r="E53">
         <v>3313</v>
       </c>
       <c r="F53" t="s">
-        <v>263</v>
+        <v>213</v>
       </c>
       <c r="G53">
         <v>16.2</v>
       </c>
       <c r="H53" t="s">
-        <v>264</v>
+        <v>214</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>265</v>
+        <v>215</v>
       </c>
       <c r="B54" t="s">
-        <v>266</v>
+        <v>216</v>
       </c>
       <c r="C54" t="s">
-        <v>168</v>
-      </c>
-      <c r="D54" t="s">
-        <v>267</v>
+        <v>137</v>
+      </c>
+      <c r="D54">
+        <v>17.649999999999999</v>
       </c>
       <c r="E54">
         <v>3577</v>
       </c>
       <c r="F54" t="s">
-        <v>188</v>
+        <v>153</v>
       </c>
       <c r="G54">
         <v>11.5</v>
       </c>
       <c r="H54" t="s">
-        <v>268</v>
+        <v>217</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>269</v>
+        <v>218</v>
       </c>
       <c r="B55" t="s">
-        <v>270</v>
+        <v>219</v>
       </c>
       <c r="C55" t="s">
-        <v>183</v>
-      </c>
-      <c r="D55" t="s">
-        <v>271</v>
+        <v>149</v>
+      </c>
+      <c r="D55">
+        <v>21.01</v>
       </c>
       <c r="E55">
         <v>3314</v>
       </c>
       <c r="F55" t="s">
-        <v>272</v>
+        <v>220</v>
       </c>
       <c r="G55">
         <v>80.400000000000006</v>
       </c>
       <c r="H55" t="s">
-        <v>171</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>273</v>
+        <v>221</v>
       </c>
       <c r="B56" t="s">
-        <v>274</v>
+        <v>222</v>
       </c>
       <c r="C56" t="s">
-        <v>275</v>
-      </c>
-      <c r="D56" t="s">
-        <v>276</v>
+        <v>223</v>
+      </c>
+      <c r="D56">
+        <v>15.39</v>
       </c>
       <c r="E56">
         <v>2048</v>
       </c>
       <c r="F56" t="s">
-        <v>277</v>
+        <v>224</v>
       </c>
       <c r="G56">
         <v>26.1</v>
       </c>
       <c r="H56" t="s">
-        <v>278</v>
+        <v>225</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>279</v>
+        <v>226</v>
       </c>
       <c r="B57" t="s">
-        <v>280</v>
+        <v>227</v>
       </c>
       <c r="C57" t="s">
-        <v>90</v>
-      </c>
-      <c r="D57" t="s">
-        <v>281</v>
+        <v>75</v>
+      </c>
+      <c r="D57">
+        <v>15.73</v>
       </c>
       <c r="E57">
         <v>2265</v>
       </c>
       <c r="F57" t="s">
-        <v>282</v>
+        <v>228</v>
       </c>
       <c r="G57">
         <v>24.3</v>
       </c>
       <c r="H57" t="s">
-        <v>283</v>
+        <v>229</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>284</v>
+        <v>230</v>
       </c>
       <c r="B58" t="s">
-        <v>285</v>
+        <v>231</v>
       </c>
       <c r="C58" t="s">
-        <v>165</v>
-      </c>
-      <c r="D58" t="s">
-        <v>286</v>
+        <v>134</v>
+      </c>
+      <c r="D58">
+        <v>16.2</v>
       </c>
       <c r="E58">
         <v>1573</v>
       </c>
       <c r="F58" t="s">
-        <v>287</v>
+        <v>232</v>
       </c>
       <c r="G58">
         <v>8.4</v>
       </c>
       <c r="H58" t="s">
-        <v>288</v>
+        <v>233</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>289</v>
+        <v>234</v>
       </c>
       <c r="B59" t="s">
-        <v>290</v>
+        <v>235</v>
       </c>
       <c r="C59" t="s">
-        <v>291</v>
-      </c>
-      <c r="D59" t="s">
-        <v>111</v>
+        <v>236</v>
+      </c>
+      <c r="D59">
+        <v>18.079999999999998</v>
       </c>
       <c r="E59">
         <v>3973</v>
       </c>
       <c r="F59" t="s">
-        <v>292</v>
+        <v>237</v>
       </c>
       <c r="G59">
         <v>327.5</v>
       </c>
       <c r="H59" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>293</v>
+        <v>238</v>
       </c>
       <c r="B60" t="s">
-        <v>294</v>
+        <v>239</v>
       </c>
       <c r="C60" t="s">
-        <v>99</v>
-      </c>
-      <c r="D60" t="s">
-        <v>295</v>
+        <v>82</v>
+      </c>
+      <c r="D60">
+        <v>13.87</v>
       </c>
       <c r="E60">
         <v>3923</v>
       </c>
       <c r="F60" t="s">
-        <v>296</v>
+        <v>240</v>
       </c>
       <c r="G60">
         <v>21.9</v>
       </c>
       <c r="H60" t="s">
-        <v>297</v>
+        <v>241</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>298</v>
+        <v>242</v>
       </c>
       <c r="B61" t="s">
-        <v>299</v>
+        <v>243</v>
       </c>
       <c r="C61" t="s">
-        <v>96</v>
-      </c>
-      <c r="D61" t="s">
-        <v>300</v>
+        <v>80</v>
+      </c>
+      <c r="D61">
+        <v>16.850000000000001</v>
       </c>
       <c r="E61">
         <v>2859</v>
       </c>
       <c r="F61" t="s">
-        <v>301</v>
+        <v>244</v>
       </c>
       <c r="G61">
         <v>21.4</v>
       </c>
       <c r="H61" t="s">
-        <v>302</v>
+        <v>245</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>303</v>
+        <v>246</v>
       </c>
       <c r="B62" t="s">
-        <v>304</v>
+        <v>247</v>
       </c>
       <c r="C62" t="s">
         <v>3</v>
       </c>
-      <c r="D62" t="s">
-        <v>305</v>
+      <c r="D62">
+        <v>10.88</v>
       </c>
       <c r="E62">
         <v>4736</v>
       </c>
       <c r="F62" t="s">
-        <v>306</v>
+        <v>248</v>
       </c>
       <c r="G62">
         <v>15.9</v>
       </c>
       <c r="H62" t="s">
-        <v>307</v>
+        <v>249</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>308</v>
+        <v>250</v>
       </c>
       <c r="B63" t="s">
-        <v>309</v>
+        <v>251</v>
       </c>
       <c r="C63" t="s">
-        <v>96</v>
-      </c>
-      <c r="D63" t="s">
-        <v>310</v>
+        <v>80</v>
+      </c>
+      <c r="D63">
+        <v>13.59</v>
       </c>
       <c r="E63">
         <v>4663</v>
       </c>
       <c r="F63" t="s">
-        <v>311</v>
+        <v>252</v>
       </c>
       <c r="G63">
         <v>210.4</v>
       </c>
       <c r="H63" t="s">
-        <v>312</v>
+        <v>253</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>313</v>
+        <v>254</v>
       </c>
       <c r="B64" t="s">
-        <v>314</v>
+        <v>255</v>
       </c>
       <c r="C64" t="s">
-        <v>165</v>
-      </c>
-      <c r="D64" t="s">
-        <v>315</v>
+        <v>134</v>
+      </c>
+      <c r="D64">
+        <v>13.88</v>
       </c>
       <c r="E64">
         <v>3719</v>
       </c>
       <c r="F64" t="s">
-        <v>316</v>
+        <v>256</v>
       </c>
       <c r="G64">
         <v>58.4</v>
       </c>
       <c r="H64" t="s">
-        <v>297</v>
+        <v>241</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>317</v>
+        <v>257</v>
       </c>
       <c r="B65" t="s">
-        <v>318</v>
+        <v>258</v>
       </c>
       <c r="C65" t="s">
-        <v>319</v>
-      </c>
-      <c r="D65" t="s">
-        <v>320</v>
+        <v>259</v>
+      </c>
+      <c r="D65">
+        <v>17.260000000000002</v>
       </c>
       <c r="E65">
         <v>3547</v>
       </c>
       <c r="F65" t="s">
-        <v>321</v>
+        <v>260</v>
       </c>
       <c r="G65">
         <v>91.8</v>
       </c>
       <c r="H65" t="s">
-        <v>322</v>
+        <v>261</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>323</v>
+        <v>262</v>
       </c>
       <c r="B66" t="s">
-        <v>324</v>
+        <v>263</v>
       </c>
       <c r="C66" t="s">
-        <v>9</v>
-      </c>
-      <c r="D66" t="s">
-        <v>325</v>
+        <v>8</v>
+      </c>
+      <c r="D66">
+        <v>14.2</v>
       </c>
       <c r="E66">
         <v>5123</v>
       </c>
       <c r="F66" t="s">
-        <v>326</v>
+        <v>264</v>
       </c>
       <c r="G66">
         <v>37</v>
       </c>
       <c r="H66" t="s">
-        <v>327</v>
+        <v>265</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>328</v>
+        <v>266</v>
       </c>
       <c r="B67" t="s">
-        <v>329</v>
+        <v>267</v>
       </c>
       <c r="C67" t="s">
-        <v>165</v>
-      </c>
-      <c r="D67" t="s">
-        <v>330</v>
+        <v>134</v>
+      </c>
+      <c r="D67">
+        <v>14.17</v>
       </c>
       <c r="E67">
         <v>2996</v>
       </c>
       <c r="F67" t="s">
-        <v>331</v>
+        <v>268</v>
       </c>
       <c r="G67">
         <v>38.1</v>
       </c>
       <c r="H67" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>332</v>
+        <v>269</v>
       </c>
       <c r="B68" t="s">
-        <v>333</v>
+        <v>270</v>
       </c>
       <c r="C68" t="s">
-        <v>39</v>
-      </c>
-      <c r="D68" t="s">
-        <v>334</v>
+        <v>33</v>
+      </c>
+      <c r="D68">
+        <v>26.58</v>
       </c>
       <c r="E68">
         <v>19592</v>
       </c>
       <c r="F68" t="s">
-        <v>335</v>
+        <v>271</v>
       </c>
       <c r="G68">
         <v>257.5</v>
       </c>
       <c r="H68" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>336</v>
+        <v>272</v>
       </c>
       <c r="B69" t="s">
-        <v>337</v>
+        <v>273</v>
       </c>
       <c r="C69" t="s">
-        <v>338</v>
-      </c>
-      <c r="D69" t="s">
-        <v>339</v>
+        <v>274</v>
+      </c>
+      <c r="D69">
+        <v>21.02</v>
       </c>
       <c r="E69">
         <v>2969</v>
       </c>
       <c r="F69" t="s">
-        <v>340</v>
+        <v>275</v>
       </c>
       <c r="G69">
         <v>42.5</v>
       </c>
       <c r="H69" t="s">
-        <v>341</v>
+        <v>276</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>342</v>
+        <v>277</v>
       </c>
       <c r="B70" t="s">
-        <v>343</v>
+        <v>278</v>
       </c>
       <c r="C70" t="s">
-        <v>319</v>
-      </c>
-      <c r="D70" t="s">
-        <v>344</v>
+        <v>259</v>
+      </c>
+      <c r="D70">
+        <v>19.329999999999998</v>
       </c>
       <c r="E70">
         <v>6907</v>
       </c>
       <c r="F70" t="s">
-        <v>345</v>
+        <v>279</v>
       </c>
       <c r="G70">
         <v>80.3</v>
       </c>
       <c r="H70" t="s">
-        <v>158</v>
+        <v>129</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>346</v>
+        <v>280</v>
       </c>
       <c r="B71" t="s">
-        <v>347</v>
+        <v>281</v>
       </c>
       <c r="C71" t="s">
-        <v>12</v>
-      </c>
-      <c r="D71" t="s">
-        <v>237</v>
+        <v>10</v>
+      </c>
+      <c r="D71">
+        <v>19.260000000000002</v>
       </c>
       <c r="E71">
         <v>2933</v>
       </c>
       <c r="F71" t="s">
-        <v>348</v>
+        <v>282</v>
       </c>
       <c r="G71">
         <v>15.2</v>
       </c>
       <c r="H71" t="s">
-        <v>349</v>
+        <v>283</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>350</v>
+        <v>284</v>
       </c>
       <c r="B72" t="s">
-        <v>351</v>
+        <v>285</v>
       </c>
       <c r="C72" t="s">
-        <v>352</v>
-      </c>
-      <c r="D72" t="s">
-        <v>353</v>
+        <v>286</v>
+      </c>
+      <c r="D72">
+        <v>18.38</v>
       </c>
       <c r="E72">
         <v>3665</v>
       </c>
       <c r="F72" t="s">
-        <v>354</v>
+        <v>287</v>
       </c>
       <c r="G72">
         <v>34.799999999999997</v>
       </c>
       <c r="H72" t="s">
-        <v>355</v>
+        <v>288</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>356</v>
+        <v>289</v>
       </c>
       <c r="B73" t="s">
-        <v>357</v>
+        <v>290</v>
       </c>
       <c r="C73" t="s">
-        <v>358</v>
-      </c>
-      <c r="D73" t="s">
-        <v>359</v>
+        <v>291</v>
+      </c>
+      <c r="D73">
+        <v>17.38</v>
       </c>
       <c r="E73">
         <v>3089</v>
       </c>
       <c r="F73" t="s">
-        <v>360</v>
+        <v>292</v>
       </c>
       <c r="G73">
         <v>122.4</v>
       </c>
       <c r="H73" t="s">
-        <v>361</v>
+        <v>293</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>362</v>
+        <v>294</v>
       </c>
       <c r="B74" t="s">
-        <v>363</v>
+        <v>295</v>
       </c>
       <c r="C74" t="s">
-        <v>364</v>
-      </c>
-      <c r="D74" t="s">
-        <v>365</v>
+        <v>296</v>
+      </c>
+      <c r="D74">
+        <v>24.33</v>
       </c>
       <c r="E74">
         <v>11900</v>
       </c>
       <c r="F74" t="s">
-        <v>366</v>
+        <v>297</v>
       </c>
       <c r="G74">
         <v>60</v>
       </c>
       <c r="H74" t="s">
-        <v>367</v>
+        <v>298</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>368</v>
+        <v>299</v>
       </c>
       <c r="B75" t="s">
-        <v>369</v>
+        <v>300</v>
       </c>
       <c r="C75" t="s">
-        <v>370</v>
-      </c>
-      <c r="D75" t="s">
-        <v>371</v>
+        <v>301</v>
+      </c>
+      <c r="D75">
+        <v>16.920000000000002</v>
       </c>
       <c r="E75">
         <v>3433</v>
       </c>
       <c r="F75" t="s">
-        <v>372</v>
+        <v>302</v>
       </c>
       <c r="G75">
         <v>44.2</v>
       </c>
       <c r="H75" t="s">
-        <v>264</v>
+        <v>214</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>373</v>
+        <v>303</v>
       </c>
       <c r="B76" t="s">
-        <v>374</v>
+        <v>304</v>
       </c>
       <c r="C76" t="s">
-        <v>90</v>
-      </c>
-      <c r="D76" t="s">
-        <v>375</v>
+        <v>75</v>
+      </c>
+      <c r="D76">
+        <v>21.88</v>
       </c>
       <c r="E76">
         <v>6340</v>
       </c>
       <c r="F76" t="s">
-        <v>376</v>
+        <v>305</v>
       </c>
       <c r="G76">
         <v>31</v>
       </c>
       <c r="H76" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>